<commit_message>
Repeated and redudnat files deleted Project description updated (README.md) Chemical analysys script updated (scripts/) Chemical analysis input files added (input_data/)
</commit_message>
<xml_diff>
--- a/input_data/chemical_data_manuscript_1.xlsx
+++ b/input_data/chemical_data_manuscript_1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE06670F-A2FB-47C7-90C2-35949104BC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714148E1-8B4A-418E-AB17-700AFC55D0AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -316,7 +316,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -606,7 +616,7 @@
   <dimension ref="A1:AD33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T33" sqref="E2:T33"/>
+      <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2739,11 +2749,6 @@
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="E2:T33">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
-      <formula>30</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>